<commit_message>
Heuristic initial structure Solver input definition
</commit_message>
<xml_diff>
--- a/Input example files/Requests.xlsx
+++ b/Input example files/Requests.xlsx
@@ -186,9 +186,6 @@
     <t>JRO</t>
   </si>
   <si>
-    <t>SSK</t>
-  </si>
-  <si>
     <t>LOB</t>
   </si>
   <si>
@@ -481,6 +478,9 @@
   </si>
   <si>
     <t>Q3</t>
+  </si>
+  <si>
+    <t>GBE</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,7 @@
   <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -893,7 +893,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="G2" t="s">
         <v>51</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>13</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>13</v>
@@ -1093,7 +1093,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="G7" t="s">
         <v>51</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>14</v>
@@ -1130,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="G8" t="s">
         <v>51</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>14</v>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="G9" t="s">
         <v>51</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>14</v>
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="G10" t="s">
         <v>51</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>14</v>
@@ -1241,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="G11" t="s">
         <v>51</v>
@@ -1278,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
         <v>54</v>
@@ -1300,7 +1300,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>15</v>
@@ -1315,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
         <v>54</v>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="4">
         <v>22025947</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="4">
         <v>22025947</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="4">
         <v>22025947</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="4">
         <v>22025947</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>16</v>
@@ -1500,10 +1500,10 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" si="0"/>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>16</v>
@@ -1537,10 +1537,10 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H19" s="6">
         <f t="shared" si="0"/>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>16</v>
@@ -1574,10 +1574,10 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G20" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H20" s="6">
         <f t="shared" si="0"/>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>16</v>
@@ -1611,10 +1611,10 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H21" s="6">
         <f t="shared" si="0"/>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>16</v>
@@ -1648,10 +1648,10 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H22" s="6">
         <f t="shared" si="0"/>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>16</v>
@@ -1685,10 +1685,10 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H23" s="6">
         <f t="shared" si="0"/>
@@ -1722,10 +1722,10 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H24" s="6">
         <f t="shared" si="0"/>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>16</v>
@@ -1759,10 +1759,10 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G25" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H25" s="6">
         <f t="shared" si="0"/>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>17</v>
@@ -1796,10 +1796,10 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" si="0"/>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>18</v>
@@ -1833,7 +1833,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G27" t="s">
         <v>51</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>18</v>
@@ -1870,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G28" t="s">
         <v>51</v>
@@ -1892,7 +1892,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>18</v>
@@ -1907,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G29" t="s">
         <v>51</v>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>18</v>
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G30" t="s">
         <v>51</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>19</v>
@@ -1984,7 +1984,7 @@
         <v>51</v>
       </c>
       <c r="G31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H31" s="6">
         <f t="shared" si="0"/>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>19</v>
@@ -2021,7 +2021,7 @@
         <v>51</v>
       </c>
       <c r="G32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H32" s="6">
         <f t="shared" si="0"/>
@@ -2040,7 +2040,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>19</v>
@@ -2058,7 +2058,7 @@
         <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H33" s="6">
         <f t="shared" si="0"/>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>19</v>
@@ -2095,7 +2095,7 @@
         <v>51</v>
       </c>
       <c r="G34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H34" s="6">
         <f t="shared" si="0"/>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>20</v>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>20</v>
@@ -2188,7 +2188,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>21</v>
@@ -2206,7 +2206,7 @@
         <v>51</v>
       </c>
       <c r="G37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H37" s="6">
         <f t="shared" si="0"/>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>21</v>
@@ -2243,7 +2243,7 @@
         <v>51</v>
       </c>
       <c r="G38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H38" s="6">
         <f t="shared" si="0"/>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>22</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>22</v>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>22</v>
@@ -2373,7 +2373,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>22</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>23</v>
@@ -2428,7 +2428,7 @@
         <v>53</v>
       </c>
       <c r="G43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H43" s="6">
         <f t="shared" si="0"/>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>23</v>
@@ -2465,7 +2465,7 @@
         <v>53</v>
       </c>
       <c r="G44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H44" s="6">
         <f t="shared" si="0"/>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>24</v>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>24</v>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>25</v>
@@ -2576,7 +2576,7 @@
         <v>53</v>
       </c>
       <c r="G47" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H47" s="6">
         <f t="shared" si="0"/>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>25</v>
@@ -2613,7 +2613,7 @@
         <v>53</v>
       </c>
       <c r="G48" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H48" s="6">
         <f t="shared" si="0"/>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>25</v>
@@ -2650,7 +2650,7 @@
         <v>53</v>
       </c>
       <c r="G49" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H49" s="6">
         <f t="shared" si="0"/>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>25</v>
@@ -2687,7 +2687,7 @@
         <v>53</v>
       </c>
       <c r="G50" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H50" s="6">
         <f t="shared" si="0"/>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>26</v>
@@ -2721,7 +2721,7 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="G51" t="s">
         <v>54</v>
@@ -2743,7 +2743,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>27</v>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>27</v>
@@ -2817,7 +2817,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>28</v>
@@ -2835,7 +2835,7 @@
         <v>53</v>
       </c>
       <c r="G54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H54" s="6">
         <f t="shared" si="0"/>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>28</v>
@@ -2872,7 +2872,7 @@
         <v>53</v>
       </c>
       <c r="G55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H55" s="6">
         <f t="shared" si="0"/>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>28</v>
@@ -2909,7 +2909,7 @@
         <v>53</v>
       </c>
       <c r="G56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H56" s="6">
         <f t="shared" si="0"/>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>28</v>
@@ -2946,7 +2946,7 @@
         <v>53</v>
       </c>
       <c r="G57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H57" s="6">
         <f t="shared" si="0"/>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>29</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>29</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>30</v>
@@ -3054,10 +3054,10 @@
         <v>1</v>
       </c>
       <c r="F60" t="s">
+        <v>153</v>
+      </c>
+      <c r="G60" t="s">
         <v>55</v>
-      </c>
-      <c r="G60" t="s">
-        <v>56</v>
       </c>
       <c r="H60" s="6">
         <f t="shared" si="0"/>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>30</v>
@@ -3091,10 +3091,10 @@
         <v>1</v>
       </c>
       <c r="F61" t="s">
+        <v>153</v>
+      </c>
+      <c r="G61" t="s">
         <v>55</v>
-      </c>
-      <c r="G61" t="s">
-        <v>56</v>
       </c>
       <c r="H61" s="6">
         <f t="shared" si="0"/>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>30</v>
@@ -3128,10 +3128,10 @@
         <v>1</v>
       </c>
       <c r="F62" t="s">
+        <v>153</v>
+      </c>
+      <c r="G62" t="s">
         <v>55</v>
-      </c>
-      <c r="G62" t="s">
-        <v>56</v>
       </c>
       <c r="H62" s="6">
         <f t="shared" si="0"/>
@@ -3150,7 +3150,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>30</v>
@@ -3165,10 +3165,10 @@
         <v>0</v>
       </c>
       <c r="F63" t="s">
+        <v>153</v>
+      </c>
+      <c r="G63" t="s">
         <v>55</v>
-      </c>
-      <c r="G63" t="s">
-        <v>56</v>
       </c>
       <c r="H63" s="6">
         <f t="shared" si="0"/>
@@ -3187,7 +3187,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>30</v>
@@ -3202,10 +3202,10 @@
         <v>1</v>
       </c>
       <c r="F64" t="s">
+        <v>153</v>
+      </c>
+      <c r="G64" t="s">
         <v>55</v>
-      </c>
-      <c r="G64" t="s">
-        <v>56</v>
       </c>
       <c r="H64" s="6">
         <f t="shared" si="0"/>
@@ -3224,7 +3224,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>30</v>
@@ -3239,10 +3239,10 @@
         <v>0</v>
       </c>
       <c r="F65" t="s">
+        <v>153</v>
+      </c>
+      <c r="G65" t="s">
         <v>55</v>
-      </c>
-      <c r="G65" t="s">
-        <v>56</v>
       </c>
       <c r="H65" s="6">
         <f t="shared" si="0"/>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>31</v>
@@ -3279,7 +3279,7 @@
         <v>51</v>
       </c>
       <c r="G66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H66" s="6">
         <f t="shared" si="0"/>
@@ -3298,7 +3298,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>32</v>
@@ -3313,7 +3313,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G67" t="s">
         <v>51</v>
@@ -3335,7 +3335,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>32</v>
@@ -3350,7 +3350,7 @@
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G68" t="s">
         <v>51</v>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>32</v>
@@ -3387,7 +3387,7 @@
         <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G69" t="s">
         <v>51</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>33</v>
@@ -3446,7 +3446,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>33</v>
@@ -3483,7 +3483,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>34</v>
@@ -3498,7 +3498,7 @@
         <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G72" t="s">
         <v>53</v>
@@ -3520,7 +3520,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>35</v>
@@ -3535,7 +3535,7 @@
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G73" t="s">
         <v>51</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>35</v>
@@ -3572,7 +3572,7 @@
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G74" t="s">
         <v>51</v>
@@ -3594,7 +3594,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>36</v>
@@ -3631,7 +3631,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>37</v>
@@ -3646,10 +3646,10 @@
         <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H76" s="6">
         <f t="shared" si="2"/>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>37</v>
@@ -3683,10 +3683,10 @@
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H77" s="6">
         <f t="shared" si="2"/>
@@ -3705,7 +3705,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>38</v>
@@ -3720,10 +3720,10 @@
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="G78" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H78" s="6">
         <f t="shared" si="2"/>
@@ -3742,7 +3742,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>38</v>
@@ -3757,10 +3757,10 @@
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="G79" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H79" s="6">
         <f t="shared" si="2"/>
@@ -3779,7 +3779,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>39</v>
@@ -3794,7 +3794,7 @@
         <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G80" t="s">
         <v>54</v>
@@ -3816,7 +3816,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>40</v>
@@ -3831,7 +3831,7 @@
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G81" t="s">
         <v>51</v>
@@ -3853,7 +3853,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>41</v>
@@ -3868,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="F82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G82" t="s">
         <v>54</v>
@@ -3890,7 +3890,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>41</v>
@@ -3905,7 +3905,7 @@
         <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G83" t="s">
         <v>54</v>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>41</v>
@@ -3942,7 +3942,7 @@
         <v>0</v>
       </c>
       <c r="F84" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G84" t="s">
         <v>54</v>
@@ -3964,7 +3964,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>41</v>
@@ -3979,7 +3979,7 @@
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G85" t="s">
         <v>54</v>
@@ -4001,7 +4001,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>41</v>
@@ -4016,7 +4016,7 @@
         <v>0</v>
       </c>
       <c r="F86" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G86" t="s">
         <v>54</v>
@@ -4038,7 +4038,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>41</v>
@@ -4053,7 +4053,7 @@
         <v>1</v>
       </c>
       <c r="F87" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G87" t="s">
         <v>54</v>
@@ -4075,7 +4075,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>42</v>
@@ -4093,7 +4093,7 @@
         <v>51</v>
       </c>
       <c r="G88" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H88" s="6">
         <f t="shared" si="2"/>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>42</v>
@@ -4130,7 +4130,7 @@
         <v>51</v>
       </c>
       <c r="G89" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H89" s="6">
         <f t="shared" si="2"/>
@@ -4149,7 +4149,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>42</v>
@@ -4167,7 +4167,7 @@
         <v>51</v>
       </c>
       <c r="G90" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H90" s="6">
         <f t="shared" si="2"/>
@@ -4186,7 +4186,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>43</v>
@@ -4201,10 +4201,10 @@
         <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G91" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H91" s="6">
         <f t="shared" si="2"/>
@@ -4223,7 +4223,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>43</v>
@@ -4238,10 +4238,10 @@
         <v>0</v>
       </c>
       <c r="F92" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G92" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H92" s="6">
         <f t="shared" si="2"/>
@@ -4260,7 +4260,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>44</v>
@@ -4278,7 +4278,7 @@
         <v>51</v>
       </c>
       <c r="G93" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="H93" s="6">
         <f t="shared" si="2"/>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>45</v>
@@ -4334,7 +4334,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Heuristic new version Input examples changes
</commit_message>
<xml_diff>
--- a/Input example files/Requests.xlsx
+++ b/Input example files/Requests.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC4C58A-4488-4583-9B04-B740EABC9DA1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Request" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="163">
   <si>
     <t>Passenger</t>
   </si>
@@ -481,6 +483,33 @@
   </si>
   <si>
     <t>GBE</t>
+  </si>
+  <si>
+    <t>CQ202</t>
+  </si>
+  <si>
+    <t>CQ232</t>
+  </si>
+  <si>
+    <t>CQ251</t>
+  </si>
+  <si>
+    <t>CQ241</t>
+  </si>
+  <si>
+    <t>CQ291</t>
+  </si>
+  <si>
+    <t>CQ262</t>
+  </si>
+  <si>
+    <t>CQ204</t>
+  </si>
+  <si>
+    <t>CQ205</t>
+  </si>
+  <si>
+    <t>CQ231</t>
   </si>
 </sst>
 </file>
@@ -842,7 +871,7 @@
   <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="G2" sqref="G2:G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4372,4 +4401,2748 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB11E71-77E4-4E18-AFFB-C5AEF4DBF4FA}">
+  <dimension ref="A1:I94"/>
+  <sheetViews>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F94"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" s="5">
+        <v>25569.420138888891</v>
+      </c>
+      <c r="I1" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="5">
+        <v>25569.600694444445</v>
+      </c>
+      <c r="I2" s="5">
+        <v>25569.708333333332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="5">
+        <v>25569.600694444445</v>
+      </c>
+      <c r="I3" s="5">
+        <v>25569.708333333332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H4" s="5">
+        <v>25569.541666666668</v>
+      </c>
+      <c r="I4" s="5">
+        <v>25569.600694444445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" s="5">
+        <v>25569.541666666668</v>
+      </c>
+      <c r="I5" s="5">
+        <v>25569.600694444445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" t="s">
+        <v>154</v>
+      </c>
+      <c r="H6" s="5">
+        <v>25569.420138888891</v>
+      </c>
+      <c r="I6" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" s="5">
+        <v>25569.420138888891</v>
+      </c>
+      <c r="I7" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>154</v>
+      </c>
+      <c r="H8" s="5">
+        <v>25569.420138888891</v>
+      </c>
+      <c r="I8" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" s="5">
+        <v>25569.420138888891</v>
+      </c>
+      <c r="I9" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" s="5">
+        <v>25569.420138888891</v>
+      </c>
+      <c r="I10" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" s="5">
+        <v>25569.40625</v>
+      </c>
+      <c r="I11" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>154</v>
+      </c>
+      <c r="H12" s="5">
+        <v>25569.40625</v>
+      </c>
+      <c r="I12" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B13" s="4">
+        <v>22025947</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>154</v>
+      </c>
+      <c r="H13" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I13" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B14" s="4">
+        <v>22025947</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>154</v>
+      </c>
+      <c r="H14" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I14" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B15" s="4">
+        <v>22025947</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I15" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B16" s="4">
+        <v>22025947</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" t="s">
+        <v>154</v>
+      </c>
+      <c r="H16" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I16" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" t="s">
+        <v>153</v>
+      </c>
+      <c r="G17" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17" s="5">
+        <v>25569.482638888891</v>
+      </c>
+      <c r="I17" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" t="s">
+        <v>157</v>
+      </c>
+      <c r="H18" s="5">
+        <v>25569.482638888891</v>
+      </c>
+      <c r="I18" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G19" t="s">
+        <v>157</v>
+      </c>
+      <c r="H19" s="5">
+        <v>25569.482638888891</v>
+      </c>
+      <c r="I19" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" t="s">
+        <v>157</v>
+      </c>
+      <c r="H20" s="5">
+        <v>25569.482638888891</v>
+      </c>
+      <c r="I20" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G21" t="s">
+        <v>157</v>
+      </c>
+      <c r="H21" s="5">
+        <v>25569.482638888891</v>
+      </c>
+      <c r="I21" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>153</v>
+      </c>
+      <c r="G22" t="s">
+        <v>157</v>
+      </c>
+      <c r="H22" s="5">
+        <v>25569.482638888891</v>
+      </c>
+      <c r="I22" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" t="s">
+        <v>153</v>
+      </c>
+      <c r="G23" t="s">
+        <v>157</v>
+      </c>
+      <c r="H23" s="5">
+        <v>25569.482638888891</v>
+      </c>
+      <c r="I23" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" t="s">
+        <v>153</v>
+      </c>
+      <c r="G24" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" s="5">
+        <v>25569.482638888891</v>
+      </c>
+      <c r="I24" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" t="s">
+        <v>157</v>
+      </c>
+      <c r="H25" s="5">
+        <v>25569.482638888891</v>
+      </c>
+      <c r="I25" s="5">
+        <v>25569.520833333332</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" t="s">
+        <v>154</v>
+      </c>
+      <c r="H26" s="5">
+        <v>25569.475694444445</v>
+      </c>
+      <c r="I26" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" t="s">
+        <v>154</v>
+      </c>
+      <c r="H27" s="5">
+        <v>25569.475694444445</v>
+      </c>
+      <c r="I27" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" s="5">
+        <v>25569.475694444445</v>
+      </c>
+      <c r="I28" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" t="s">
+        <v>154</v>
+      </c>
+      <c r="H29" s="5">
+        <v>25569.475694444445</v>
+      </c>
+      <c r="I29" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" t="s">
+        <v>156</v>
+      </c>
+      <c r="H30" s="5">
+        <v>25569.541666666668</v>
+      </c>
+      <c r="I30" s="5">
+        <v>25569.652777777777</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" t="s">
+        <v>156</v>
+      </c>
+      <c r="H31" s="5">
+        <v>25569.541666666668</v>
+      </c>
+      <c r="I31" s="5">
+        <v>25569.652777777777</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" t="s">
+        <v>156</v>
+      </c>
+      <c r="H32" s="5">
+        <v>25569.541666666668</v>
+      </c>
+      <c r="I32" s="5">
+        <v>25569.652777777777</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" t="s">
+        <v>156</v>
+      </c>
+      <c r="H33" s="5">
+        <v>25569.541666666668</v>
+      </c>
+      <c r="I33" s="5">
+        <v>25569.652777777777</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" t="s">
+        <v>154</v>
+      </c>
+      <c r="H34" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I34" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" t="s">
+        <v>154</v>
+      </c>
+      <c r="H35" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I35" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" t="s">
+        <v>57</v>
+      </c>
+      <c r="G36" t="s">
+        <v>156</v>
+      </c>
+      <c r="H36" s="5">
+        <v>25569.541666666668</v>
+      </c>
+      <c r="I36" s="5">
+        <v>25569.631944444445</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" t="s">
+        <v>156</v>
+      </c>
+      <c r="H37" s="5">
+        <v>25569.541666666668</v>
+      </c>
+      <c r="I37" s="5">
+        <v>25569.631944444445</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" t="s">
+        <v>154</v>
+      </c>
+      <c r="H38" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I38" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" t="s">
+        <v>154</v>
+      </c>
+      <c r="H39" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I39" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G40" t="s">
+        <v>154</v>
+      </c>
+      <c r="H40" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I40" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41" t="s">
+        <v>51</v>
+      </c>
+      <c r="G41" t="s">
+        <v>154</v>
+      </c>
+      <c r="H41" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I41" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" t="s">
+        <v>158</v>
+      </c>
+      <c r="H42" s="5">
+        <v>25569.375</v>
+      </c>
+      <c r="I42" s="5">
+        <v>25569.420138888891</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" t="s">
+        <v>57</v>
+      </c>
+      <c r="G43" t="s">
+        <v>158</v>
+      </c>
+      <c r="H43" s="5">
+        <v>25569.375</v>
+      </c>
+      <c r="I43" s="5">
+        <v>25569.420138888891</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G44" t="s">
+        <v>154</v>
+      </c>
+      <c r="H44" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I44" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F45" t="s">
+        <v>51</v>
+      </c>
+      <c r="G45" t="s">
+        <v>154</v>
+      </c>
+      <c r="H45" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I45" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" t="s">
+        <v>53</v>
+      </c>
+      <c r="F46" t="s">
+        <v>153</v>
+      </c>
+      <c r="G46" t="s">
+        <v>158</v>
+      </c>
+      <c r="H46" s="5">
+        <v>25569.375</v>
+      </c>
+      <c r="I46" s="5">
+        <v>25569.385416666668</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G47" t="s">
+        <v>158</v>
+      </c>
+      <c r="H47" s="5">
+        <v>25569.375</v>
+      </c>
+      <c r="I47" s="5">
+        <v>25569.385416666668</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
+        <v>48</v>
+      </c>
+      <c r="E48" t="s">
+        <v>53</v>
+      </c>
+      <c r="F48" t="s">
+        <v>153</v>
+      </c>
+      <c r="G48" t="s">
+        <v>158</v>
+      </c>
+      <c r="H48" s="5">
+        <v>25569.375</v>
+      </c>
+      <c r="I48" s="5">
+        <v>25569.385416666668</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" t="s">
+        <v>48</v>
+      </c>
+      <c r="E49" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" t="s">
+        <v>153</v>
+      </c>
+      <c r="G49" t="s">
+        <v>158</v>
+      </c>
+      <c r="H49" s="5">
+        <v>25569.375</v>
+      </c>
+      <c r="I49" s="5">
+        <v>25569.385416666668</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>153</v>
+      </c>
+      <c r="F50" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" t="s">
+        <v>159</v>
+      </c>
+      <c r="H50" s="5">
+        <v>25569.666666666668</v>
+      </c>
+      <c r="I50" s="5">
+        <v>25569.770833333332</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" t="s">
+        <v>53</v>
+      </c>
+      <c r="F51" t="s">
+        <v>51</v>
+      </c>
+      <c r="G51" t="s">
+        <v>154</v>
+      </c>
+      <c r="H51" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I51" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" t="s">
+        <v>47</v>
+      </c>
+      <c r="D52" t="s">
+        <v>48</v>
+      </c>
+      <c r="E52" t="s">
+        <v>53</v>
+      </c>
+      <c r="F52" t="s">
+        <v>51</v>
+      </c>
+      <c r="G52" t="s">
+        <v>154</v>
+      </c>
+      <c r="H52" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I52" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" t="s">
+        <v>48</v>
+      </c>
+      <c r="E53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" t="s">
+        <v>58</v>
+      </c>
+      <c r="G53" t="s">
+        <v>160</v>
+      </c>
+      <c r="H53" s="5">
+        <v>25569.375</v>
+      </c>
+      <c r="I53" s="5">
+        <v>25569.475694444445</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" t="s">
+        <v>58</v>
+      </c>
+      <c r="G54" t="s">
+        <v>160</v>
+      </c>
+      <c r="H54" s="5">
+        <v>25569.375</v>
+      </c>
+      <c r="I54" s="5">
+        <v>25569.475694444445</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D55" t="s">
+        <v>48</v>
+      </c>
+      <c r="E55" t="s">
+        <v>53</v>
+      </c>
+      <c r="F55" t="s">
+        <v>58</v>
+      </c>
+      <c r="G55" t="s">
+        <v>160</v>
+      </c>
+      <c r="H55" s="5">
+        <v>25569.375</v>
+      </c>
+      <c r="I55" s="5">
+        <v>25569.475694444445</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" t="s">
+        <v>49</v>
+      </c>
+      <c r="E56" t="s">
+        <v>53</v>
+      </c>
+      <c r="F56" t="s">
+        <v>58</v>
+      </c>
+      <c r="G56" t="s">
+        <v>160</v>
+      </c>
+      <c r="H56" s="5">
+        <v>25569.375</v>
+      </c>
+      <c r="I56" s="5">
+        <v>25569.475694444445</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" t="s">
+        <v>53</v>
+      </c>
+      <c r="F57" t="s">
+        <v>51</v>
+      </c>
+      <c r="G57" t="s">
+        <v>154</v>
+      </c>
+      <c r="H57" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I57" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" t="s">
+        <v>47</v>
+      </c>
+      <c r="D58" t="s">
+        <v>49</v>
+      </c>
+      <c r="E58" t="s">
+        <v>53</v>
+      </c>
+      <c r="F58" t="s">
+        <v>51</v>
+      </c>
+      <c r="G58" t="s">
+        <v>154</v>
+      </c>
+      <c r="H58" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I58" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" t="s">
+        <v>48</v>
+      </c>
+      <c r="E59" t="s">
+        <v>153</v>
+      </c>
+      <c r="F59" t="s">
+        <v>55</v>
+      </c>
+      <c r="G59" t="s">
+        <v>158</v>
+      </c>
+      <c r="H59" s="5">
+        <v>25569.385416666668</v>
+      </c>
+      <c r="I59" s="5">
+        <v>25569.40625</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" t="s">
+        <v>50</v>
+      </c>
+      <c r="E60" t="s">
+        <v>153</v>
+      </c>
+      <c r="F60" t="s">
+        <v>55</v>
+      </c>
+      <c r="G60" t="s">
+        <v>158</v>
+      </c>
+      <c r="H60" s="5">
+        <v>25569.385416666668</v>
+      </c>
+      <c r="I60" s="5">
+        <v>25569.40625</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" t="s">
+        <v>153</v>
+      </c>
+      <c r="F61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61" t="s">
+        <v>158</v>
+      </c>
+      <c r="H61" s="5">
+        <v>25569.385416666668</v>
+      </c>
+      <c r="I61" s="5">
+        <v>25569.40625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62" t="s">
+        <v>48</v>
+      </c>
+      <c r="E62" t="s">
+        <v>153</v>
+      </c>
+      <c r="F62" t="s">
+        <v>55</v>
+      </c>
+      <c r="G62" t="s">
+        <v>158</v>
+      </c>
+      <c r="H62" s="5">
+        <v>25569.385416666668</v>
+      </c>
+      <c r="I62" s="5">
+        <v>25569.40625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" t="s">
+        <v>48</v>
+      </c>
+      <c r="E63" t="s">
+        <v>153</v>
+      </c>
+      <c r="F63" t="s">
+        <v>55</v>
+      </c>
+      <c r="G63" t="s">
+        <v>158</v>
+      </c>
+      <c r="H63" s="5">
+        <v>25569.385416666668</v>
+      </c>
+      <c r="I63" s="5">
+        <v>25569.40625</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" t="s">
+        <v>48</v>
+      </c>
+      <c r="E64" t="s">
+        <v>153</v>
+      </c>
+      <c r="F64" t="s">
+        <v>55</v>
+      </c>
+      <c r="G64" t="s">
+        <v>158</v>
+      </c>
+      <c r="H64" s="5">
+        <v>25569.385416666668</v>
+      </c>
+      <c r="I64" s="5">
+        <v>25569.40625</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" t="s">
+        <v>47</v>
+      </c>
+      <c r="D65" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" t="s">
+        <v>51</v>
+      </c>
+      <c r="F65" t="s">
+        <v>59</v>
+      </c>
+      <c r="G65" t="s">
+        <v>157</v>
+      </c>
+      <c r="H65" s="5">
+        <v>25569.427083333332</v>
+      </c>
+      <c r="I65" s="5">
+        <v>25569.472222222223</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" t="s">
+        <v>47</v>
+      </c>
+      <c r="D66" t="s">
+        <v>49</v>
+      </c>
+      <c r="E66" t="s">
+        <v>61</v>
+      </c>
+      <c r="F66" t="s">
+        <v>51</v>
+      </c>
+      <c r="G66" t="s">
+        <v>154</v>
+      </c>
+      <c r="H66" s="5">
+        <v>25569.475694444445</v>
+      </c>
+      <c r="I66" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" t="s">
+        <v>47</v>
+      </c>
+      <c r="D67" t="s">
+        <v>48</v>
+      </c>
+      <c r="E67" t="s">
+        <v>61</v>
+      </c>
+      <c r="F67" t="s">
+        <v>51</v>
+      </c>
+      <c r="G67" t="s">
+        <v>154</v>
+      </c>
+      <c r="H67" s="5">
+        <v>25569.475694444445</v>
+      </c>
+      <c r="I67" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" t="s">
+        <v>49</v>
+      </c>
+      <c r="E68" t="s">
+        <v>61</v>
+      </c>
+      <c r="F68" t="s">
+        <v>51</v>
+      </c>
+      <c r="G68" t="s">
+        <v>154</v>
+      </c>
+      <c r="H68" s="5">
+        <v>25569.475694444445</v>
+      </c>
+      <c r="I68" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" t="s">
+        <v>49</v>
+      </c>
+      <c r="E69" t="s">
+        <v>53</v>
+      </c>
+      <c r="F69" t="s">
+        <v>54</v>
+      </c>
+      <c r="G69" t="s">
+        <v>154</v>
+      </c>
+      <c r="H69" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I69" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" t="s">
+        <v>47</v>
+      </c>
+      <c r="D70" t="s">
+        <v>48</v>
+      </c>
+      <c r="E70" t="s">
+        <v>53</v>
+      </c>
+      <c r="F70" t="s">
+        <v>54</v>
+      </c>
+      <c r="G70" t="s">
+        <v>154</v>
+      </c>
+      <c r="H70" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I70" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" t="s">
+        <v>49</v>
+      </c>
+      <c r="E71" t="s">
+        <v>62</v>
+      </c>
+      <c r="F71" t="s">
+        <v>53</v>
+      </c>
+      <c r="G71" t="s">
+        <v>161</v>
+      </c>
+      <c r="H71" s="5">
+        <v>25569.458333333332</v>
+      </c>
+      <c r="I71" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C72" t="s">
+        <v>47</v>
+      </c>
+      <c r="D72" t="s">
+        <v>49</v>
+      </c>
+      <c r="E72" t="s">
+        <v>57</v>
+      </c>
+      <c r="F72" t="s">
+        <v>51</v>
+      </c>
+      <c r="G72" t="s">
+        <v>154</v>
+      </c>
+      <c r="H72" s="5">
+        <v>25569.392361111109</v>
+      </c>
+      <c r="I72" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" t="s">
+        <v>47</v>
+      </c>
+      <c r="D73" t="s">
+        <v>49</v>
+      </c>
+      <c r="E73" t="s">
+        <v>57</v>
+      </c>
+      <c r="F73" t="s">
+        <v>51</v>
+      </c>
+      <c r="G73" t="s">
+        <v>154</v>
+      </c>
+      <c r="H73" s="5">
+        <v>25569.392361111109</v>
+      </c>
+      <c r="I73" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C74" t="s">
+        <v>47</v>
+      </c>
+      <c r="D74" t="s">
+        <v>48</v>
+      </c>
+      <c r="E74" t="s">
+        <v>51</v>
+      </c>
+      <c r="F74" t="s">
+        <v>53</v>
+      </c>
+      <c r="G74" t="s">
+        <v>156</v>
+      </c>
+      <c r="H74" s="5">
+        <v>25569.541666666668</v>
+      </c>
+      <c r="I74" s="5">
+        <v>25569.600694444445</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C75" t="s">
+        <v>47</v>
+      </c>
+      <c r="D75" t="s">
+        <v>49</v>
+      </c>
+      <c r="E75" t="s">
+        <v>63</v>
+      </c>
+      <c r="F75" t="s">
+        <v>60</v>
+      </c>
+      <c r="G75" t="s">
+        <v>162</v>
+      </c>
+      <c r="H75" s="5">
+        <v>25569.291666666668</v>
+      </c>
+      <c r="I75" s="5">
+        <v>25569.427083333332</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" t="s">
+        <v>49</v>
+      </c>
+      <c r="E76" t="s">
+        <v>63</v>
+      </c>
+      <c r="F76" t="s">
+        <v>60</v>
+      </c>
+      <c r="G76" t="s">
+        <v>162</v>
+      </c>
+      <c r="H76" s="5">
+        <v>25569.291666666668</v>
+      </c>
+      <c r="I76" s="5">
+        <v>25569.427083333332</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" t="s">
+        <v>47</v>
+      </c>
+      <c r="D77" t="s">
+        <v>49</v>
+      </c>
+      <c r="E77" t="s">
+        <v>153</v>
+      </c>
+      <c r="F77" t="s">
+        <v>61</v>
+      </c>
+      <c r="G77" t="s">
+        <v>154</v>
+      </c>
+      <c r="H77" s="5">
+        <v>25569.420138888891</v>
+      </c>
+      <c r="I77" s="5">
+        <v>25569.475694444445</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C78" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" t="s">
+        <v>49</v>
+      </c>
+      <c r="E78" t="s">
+        <v>153</v>
+      </c>
+      <c r="F78" t="s">
+        <v>61</v>
+      </c>
+      <c r="G78" t="s">
+        <v>154</v>
+      </c>
+      <c r="H78" s="5">
+        <v>25569.420138888891</v>
+      </c>
+      <c r="I78" s="5">
+        <v>25569.475694444445</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C79" t="s">
+        <v>47</v>
+      </c>
+      <c r="D79" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" t="s">
+        <v>61</v>
+      </c>
+      <c r="F79" t="s">
+        <v>54</v>
+      </c>
+      <c r="G79" t="s">
+        <v>154</v>
+      </c>
+      <c r="H79" s="5">
+        <v>25569.475694444445</v>
+      </c>
+      <c r="I79" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" t="s">
+        <v>47</v>
+      </c>
+      <c r="D80" t="s">
+        <v>49</v>
+      </c>
+      <c r="E80" t="s">
+        <v>61</v>
+      </c>
+      <c r="F80" t="s">
+        <v>51</v>
+      </c>
+      <c r="G80" t="s">
+        <v>154</v>
+      </c>
+      <c r="H80" s="5">
+        <v>25569.475694444445</v>
+      </c>
+      <c r="I80" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C81" t="s">
+        <v>47</v>
+      </c>
+      <c r="D81" t="s">
+        <v>49</v>
+      </c>
+      <c r="E81" t="s">
+        <v>55</v>
+      </c>
+      <c r="F81" t="s">
+        <v>54</v>
+      </c>
+      <c r="G81" t="s">
+        <v>154</v>
+      </c>
+      <c r="H81" s="5">
+        <v>25569.40625</v>
+      </c>
+      <c r="I81" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C82" t="s">
+        <v>47</v>
+      </c>
+      <c r="D82" t="s">
+        <v>48</v>
+      </c>
+      <c r="E82" t="s">
+        <v>55</v>
+      </c>
+      <c r="F82" t="s">
+        <v>54</v>
+      </c>
+      <c r="G82" t="s">
+        <v>154</v>
+      </c>
+      <c r="H82" s="5">
+        <v>25569.40625</v>
+      </c>
+      <c r="I82" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C83" t="s">
+        <v>47</v>
+      </c>
+      <c r="D83" t="s">
+        <v>49</v>
+      </c>
+      <c r="E83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F83" t="s">
+        <v>54</v>
+      </c>
+      <c r="G83" t="s">
+        <v>154</v>
+      </c>
+      <c r="H83" s="5">
+        <v>25569.40625</v>
+      </c>
+      <c r="I83" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84" t="s">
+        <v>47</v>
+      </c>
+      <c r="D84" t="s">
+        <v>48</v>
+      </c>
+      <c r="E84" t="s">
+        <v>55</v>
+      </c>
+      <c r="F84" t="s">
+        <v>54</v>
+      </c>
+      <c r="G84" t="s">
+        <v>154</v>
+      </c>
+      <c r="H84" s="5">
+        <v>25569.40625</v>
+      </c>
+      <c r="I84" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C85" t="s">
+        <v>47</v>
+      </c>
+      <c r="D85" t="s">
+        <v>48</v>
+      </c>
+      <c r="E85" t="s">
+        <v>55</v>
+      </c>
+      <c r="F85" t="s">
+        <v>54</v>
+      </c>
+      <c r="G85" t="s">
+        <v>154</v>
+      </c>
+      <c r="H85" s="5">
+        <v>25569.40625</v>
+      </c>
+      <c r="I85" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C86" t="s">
+        <v>47</v>
+      </c>
+      <c r="D86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E86" t="s">
+        <v>55</v>
+      </c>
+      <c r="F86" t="s">
+        <v>54</v>
+      </c>
+      <c r="G86" t="s">
+        <v>154</v>
+      </c>
+      <c r="H86" s="5">
+        <v>25569.40625</v>
+      </c>
+      <c r="I86" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" t="s">
+        <v>46</v>
+      </c>
+      <c r="D87" t="s">
+        <v>49</v>
+      </c>
+      <c r="E87" t="s">
+        <v>51</v>
+      </c>
+      <c r="F87" t="s">
+        <v>59</v>
+      </c>
+      <c r="G87" t="s">
+        <v>157</v>
+      </c>
+      <c r="H87" s="5">
+        <v>25569.427083333332</v>
+      </c>
+      <c r="I87" s="5">
+        <v>25569.472222222223</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C88" t="s">
+        <v>46</v>
+      </c>
+      <c r="D88" t="s">
+        <v>48</v>
+      </c>
+      <c r="E88" t="s">
+        <v>51</v>
+      </c>
+      <c r="F88" t="s">
+        <v>59</v>
+      </c>
+      <c r="G88" t="s">
+        <v>157</v>
+      </c>
+      <c r="H88" s="5">
+        <v>25569.427083333332</v>
+      </c>
+      <c r="I88" s="5">
+        <v>25569.472222222223</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C89" t="s">
+        <v>46</v>
+      </c>
+      <c r="D89" t="s">
+        <v>48</v>
+      </c>
+      <c r="E89" t="s">
+        <v>51</v>
+      </c>
+      <c r="F89" t="s">
+        <v>59</v>
+      </c>
+      <c r="G89" t="s">
+        <v>157</v>
+      </c>
+      <c r="H89" s="5">
+        <v>25569.427083333332</v>
+      </c>
+      <c r="I89" s="5">
+        <v>25569.472222222223</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C90" t="s">
+        <v>47</v>
+      </c>
+      <c r="D90" t="s">
+        <v>48</v>
+      </c>
+      <c r="E90" t="s">
+        <v>61</v>
+      </c>
+      <c r="F90" t="s">
+        <v>57</v>
+      </c>
+      <c r="G90" t="s">
+        <v>156</v>
+      </c>
+      <c r="H90" s="5">
+        <v>25569.569444444445</v>
+      </c>
+      <c r="I90" s="5">
+        <v>25569.631944444445</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C91" t="s">
+        <v>47</v>
+      </c>
+      <c r="D91" t="s">
+        <v>49</v>
+      </c>
+      <c r="E91" t="s">
+        <v>61</v>
+      </c>
+      <c r="F91" t="s">
+        <v>57</v>
+      </c>
+      <c r="G91" t="s">
+        <v>156</v>
+      </c>
+      <c r="H91" s="5">
+        <v>25569.569444444445</v>
+      </c>
+      <c r="I91" s="5">
+        <v>25569.631944444445</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C92" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" t="s">
+        <v>49</v>
+      </c>
+      <c r="E92" t="s">
+        <v>51</v>
+      </c>
+      <c r="F92" t="s">
+        <v>153</v>
+      </c>
+      <c r="G92" t="s">
+        <v>157</v>
+      </c>
+      <c r="H92" s="5">
+        <v>25569.427083333332</v>
+      </c>
+      <c r="I92" s="5">
+        <v>25569.541666666668</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C93" t="s">
+        <v>47</v>
+      </c>
+      <c r="D93" t="s">
+        <v>49</v>
+      </c>
+      <c r="E93" t="s">
+        <v>53</v>
+      </c>
+      <c r="F93" t="s">
+        <v>51</v>
+      </c>
+      <c r="G93" t="s">
+        <v>154</v>
+      </c>
+      <c r="H93" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I93" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="5">
+        <v>42887</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C94" t="s">
+        <v>47</v>
+      </c>
+      <c r="D94" t="s">
+        <v>48</v>
+      </c>
+      <c r="E94" t="s">
+        <v>53</v>
+      </c>
+      <c r="F94" t="s">
+        <v>51</v>
+      </c>
+      <c r="G94" t="s">
+        <v>154</v>
+      </c>
+      <c r="H94" s="5">
+        <v>25569.447916666668</v>
+      </c>
+      <c r="I94" s="5">
+        <v>25569.489583333332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>